<commit_message>
update contents of documents.
</commit_message>
<xml_diff>
--- a/Hangman Documents/Hangman Assignment - maunal testing.xlsx
+++ b/Hangman Documents/Hangman Assignment - maunal testing.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Gareth\Gareth\Hangman Assignment\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\git\repository\Hangman Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1676,8 +1676,8 @@
       <c r="H34" s="39"/>
     </row>
   </sheetData>
-  <pageMargins left="0.31496062992125984" right="0.31496062992125984" top="0.15748031496062992" bottom="0.15748031496062992" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup paperSize="9" scale="42" fitToHeight="0" orientation="landscape" r:id="rId1"/>
+  <pageMargins left="0.11811023622047245" right="0.11811023622047245" top="0.15748031496062992" bottom="0.15748031496062992" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup paperSize="9" scale="44" fitToHeight="0" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>